<commit_message>
actualizacion etiquetas e incorporacion tipo_var
</commit_message>
<xml_diff>
--- a/document/Etiquetas.xlsx
+++ b/document/Etiquetas.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\ML_PS2_Falcone_Morales_Riverti\document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Dropbox\Facultad\UBA\Tercer trimestre\Machine Learning\ML_PS2_Falcone_Morales_Riverti\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36DD29E-3D1E-4149-B5BE-F3AAFD1F183A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0E7CA2-B625-467B-84CA-17754D598315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="607">
   <si>
     <r>
       <rPr>
@@ -848,6 +861,16 @@
         <rFont val="Trebuchet MS"/>
         <family val="2"/>
       </rPr>
+      <t>P6210s1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
       <t>Grado escolar aprobado</t>
     </r>
   </si>
@@ -6582,6 +6605,16 @@
         <rFont val="Trebuchet MS"/>
         <family val="2"/>
       </rPr>
+      <t>P5090</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
       <t>La vivienda ocupada por este hogar es:</t>
     </r>
   </si>
@@ -6661,6 +6694,16 @@
         <rFont val="Trebuchet MS"/>
         <family val="2"/>
       </rPr>
+      <t>P5130</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
       <t>Si tuviera que pagar arriendo por esta vivienda, ¿cuánto estima que tendría que pagar mensualmente?</t>
     </r>
   </si>
@@ -6740,6 +6783,16 @@
         <rFont val="Trebuchet MS"/>
         <family val="2"/>
       </rPr>
+      <t>Nper</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
       <t>Personas en el hogar</t>
     </r>
   </si>
@@ -6770,6 +6823,16 @@
         <rFont val="Trebuchet MS"/>
         <family val="2"/>
       </rPr>
+      <t>Npersug</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
       <t>Número de personas en la unidad de gasto</t>
     </r>
   </si>
@@ -7130,29 +7193,56 @@
     <t>EN ROJO COLUMNAS QUE USAMOS</t>
   </si>
   <si>
-    <t>Npersug</t>
-  </si>
-  <si>
-    <t>Nper</t>
-  </si>
-  <si>
-    <t>P6210s1</t>
-  </si>
-  <si>
-    <t>Depto</t>
-  </si>
-  <si>
-    <t>P5130</t>
-  </si>
-  <si>
-    <t>P5090</t>
+    <t>EN VERDE VARIABLES EXPLICADAS</t>
+  </si>
+  <si>
+    <t>Promedio_Educacion</t>
+  </si>
+  <si>
+    <t>hacinamiento</t>
+  </si>
+  <si>
+    <t>capacitacion_financiera</t>
+  </si>
+  <si>
+    <t>jefe_sex</t>
+  </si>
+  <si>
+    <t>Promedio de años de educacion por hogar</t>
+  </si>
+  <si>
+    <t>Promedio de dormitorios por integrante del hogar</t>
+  </si>
+  <si>
+    <t>Dummie si el individuo tiene capacitacion financiera</t>
+  </si>
+  <si>
+    <t>Dummie si el jefe de hogar es varon o mujer</t>
+  </si>
+  <si>
+    <t>Promedio_Edad</t>
+  </si>
+  <si>
+    <t>Edad promedio del hogar</t>
+  </si>
+  <si>
+    <t>Porcentaje_Sin_Jubilacion</t>
+  </si>
+  <si>
+    <t>Porcentaje_Ocupados</t>
+  </si>
+  <si>
+    <t>Porcentaje de ocupados por hogar</t>
+  </si>
+  <si>
+    <t>Porcentaje sin aportes por hogar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -7205,8 +7295,20 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -7237,6 +7339,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -7320,7 +7428,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -7387,17 +7495,32 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8108,89 +8231,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P145"/>
+  <dimension ref="A1:AB145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="34.44140625" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="6" max="6" width="43.109375" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="34.5" customWidth="1"/>
+    <col min="4" max="4" width="9.5" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="6" max="6" width="43.1640625" customWidth="1"/>
     <col min="7" max="7" width="2.6640625" customWidth="1"/>
     <col min="10" max="10" width="6.6640625" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" customWidth="1"/>
-    <col min="12" max="12" width="34.44140625" customWidth="1"/>
-    <col min="13" max="13" width="9.44140625" customWidth="1"/>
-    <col min="14" max="14" width="10.77734375" customWidth="1"/>
-    <col min="15" max="15" width="43.109375" customWidth="1"/>
+    <col min="11" max="11" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="34.5" customWidth="1"/>
+    <col min="13" max="13" width="9.5" customWidth="1"/>
+    <col min="14" max="14" width="10.83203125" customWidth="1"/>
+    <col min="15" max="15" width="43.1640625" customWidth="1"/>
     <col min="16" max="16" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="J1" s="24" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="J1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="J2" s="25" t="s">
-        <v>518</v>
-      </c>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-    </row>
-    <row r="3" spans="1:16" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="J2" s="27" t="s">
+        <v>519</v>
+      </c>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+    </row>
+    <row r="3" spans="1:28" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="J3" s="24" t="s">
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="J3" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+    </row>
+    <row r="4" spans="1:28" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -8228,7 +8351,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -8248,7 +8371,7 @@
         <v>14</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="K5" s="5" t="s">
         <v>10</v>
@@ -8265,8 +8388,16 @@
       <c r="O5" s="5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="AA5" s="25"/>
+      <c r="AB5" s="25"/>
+    </row>
+    <row r="6" spans="1:28" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>15</v>
       </c>
@@ -8286,7 +8417,7 @@
         <v>19</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>16</v>
@@ -8304,7 +8435,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
@@ -8324,7 +8455,7 @@
         <v>23</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>34</v>
@@ -8341,8 +8472,13 @@
       <c r="O7" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="S7" s="24"/>
+      <c r="T7" s="24"/>
+      <c r="U7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="24"/>
+    </row>
+    <row r="8" spans="1:28" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
@@ -8363,7 +8499,7 @@
       </c>
       <c r="H8" s="18"/>
       <c r="J8" s="7" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="K8" s="17" t="s">
         <v>25</v>
@@ -8380,8 +8516,13 @@
       <c r="O8" s="7" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="S8" s="24"/>
+      <c r="T8" s="24"/>
+      <c r="U8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+    </row>
+    <row r="9" spans="1:28" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
@@ -8401,7 +8542,7 @@
         <v>32</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="K9" s="17" t="s">
         <v>30</v>
@@ -8418,8 +8559,13 @@
       <c r="O9" s="9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+    </row>
+    <row r="10" spans="1:28" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -8439,13 +8585,13 @@
         <v>35</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="M10" s="7" t="s">
         <v>18</v>
@@ -8454,10 +8600,10 @@
         <v>13</v>
       </c>
       <c r="O10" s="7" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" ht="39.6" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>36</v>
       </c>
@@ -8477,13 +8623,13 @@
         <v>39</v>
       </c>
       <c r="J11" s="9" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="L11" s="21" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="M11" s="9" t="s">
         <v>18</v>
@@ -8492,10 +8638,10 @@
         <v>13</v>
       </c>
       <c r="O11" s="9" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" ht="52.8" x14ac:dyDescent="0.25">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" ht="75" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>40</v>
       </c>
@@ -8515,13 +8661,13 @@
         <v>43</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="K12" s="17" t="s">
-        <v>592</v>
+        <v>533</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="M12" s="7" t="s">
         <v>18</v>
@@ -8530,17 +8676,17 @@
         <v>13</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" ht="26.4" x14ac:dyDescent="0.25">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="21" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="9" t="s">
@@ -8553,13 +8699,13 @@
         <v>47</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="M13" s="9" t="s">
         <v>12</v>
@@ -8568,10 +8714,10 @@
         <v>13</v>
       </c>
       <c r="O13" s="9" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="66" x14ac:dyDescent="0.25">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" ht="90" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>48</v>
       </c>
@@ -8591,13 +8737,13 @@
         <v>51</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>591</v>
+        <v>541</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="M14" s="7" t="s">
         <v>12</v>
@@ -8606,10 +8752,10 @@
         <v>13</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="66" x14ac:dyDescent="0.25">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" ht="90" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>52</v>
       </c>
@@ -8629,13 +8775,13 @@
         <v>55</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="M15" s="9" t="s">
         <v>12</v>
@@ -8644,10 +8790,10 @@
         <v>13</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" ht="66" x14ac:dyDescent="0.25">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" ht="90" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
         <v>56</v>
       </c>
@@ -8667,13 +8813,13 @@
         <v>59</v>
       </c>
       <c r="J16" s="7" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>588</v>
+        <v>549</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="M16" s="7" t="s">
         <v>12</v>
@@ -8682,10 +8828,10 @@
         <v>13</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="79.2" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="105" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>60</v>
       </c>
@@ -8705,13 +8851,13 @@
         <v>63</v>
       </c>
       <c r="J17" s="9" t="s">
-        <v>548</v>
+        <v>552</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>587</v>
+        <v>553</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="M17" s="9" t="s">
         <v>12</v>
@@ -8720,18 +8866,18 @@
         <v>13</v>
       </c>
       <c r="O17" s="9" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="45" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>64</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>589</v>
+        <v>65</v>
       </c>
       <c r="C18" s="21" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>12</v>
@@ -8740,16 +8886,16 @@
         <v>13</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="L18" s="7" t="s">
-        <v>552</v>
+        <v>557</v>
       </c>
       <c r="M18" s="7" t="s">
         <v>12</v>
@@ -8758,18 +8904,18 @@
         <v>13</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="66" x14ac:dyDescent="0.25">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="75" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>18</v>
@@ -8778,16 +8924,16 @@
         <v>13</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="K19" s="5" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="M19" s="5" t="s">
         <v>12</v>
@@ -8796,18 +8942,18 @@
         <v>13</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="45" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>18</v>
@@ -8816,16 +8962,16 @@
         <v>13</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J20" s="7" t="s">
-        <v>557</v>
-      </c>
-      <c r="K20" s="7" t="s">
-        <v>558</v>
+        <v>562</v>
+      </c>
+      <c r="K20" s="22" t="s">
+        <v>563</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>559</v>
+        <v>564</v>
       </c>
       <c r="M20" s="7" t="s">
         <v>12</v>
@@ -8834,18 +8980,19 @@
         <v>13</v>
       </c>
       <c r="O20" s="7" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+        <v>564</v>
+      </c>
+      <c r="R20" s="23"/>
+    </row>
+    <row r="21" spans="1:18" ht="60" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>12</v>
@@ -8854,16 +9001,16 @@
         <v>13</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="M21" s="9" t="s">
         <v>12</v>
@@ -8872,18 +9019,18 @@
         <v>13</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="105.6" x14ac:dyDescent="0.25">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="120" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>18</v>
@@ -8892,16 +9039,16 @@
         <v>13</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J22" s="7" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>564</v>
+        <v>569</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="M22" s="7" t="s">
         <v>12</v>
@@ -8910,18 +9057,18 @@
         <v>13</v>
       </c>
       <c r="O22" s="7" t="s">
-        <v>565</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="75" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>12</v>
@@ -8930,16 +9077,16 @@
         <v>13</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>566</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>567</v>
+        <v>571</v>
+      </c>
+      <c r="K23" s="22" t="s">
+        <v>572</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="M23" s="9" t="s">
         <v>18</v>
@@ -8948,18 +9095,18 @@
         <v>13</v>
       </c>
       <c r="O23" s="9" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="45" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>18</v>
@@ -8968,16 +9115,16 @@
         <v>13</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="K24" s="7" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="M24" s="7" t="s">
         <v>18</v>
@@ -8986,18 +9133,18 @@
         <v>13</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>12</v>
@@ -9006,16 +9153,16 @@
         <v>13</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
       <c r="L25" s="9" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="M25" s="9" t="s">
         <v>12</v>
@@ -9024,18 +9171,18 @@
         <v>13</v>
       </c>
       <c r="O25" s="9" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="75" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>18</v>
@@ -9044,16 +9191,16 @@
         <v>13</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J26" s="7" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="M26" s="7" t="s">
         <v>12</v>
@@ -9062,18 +9209,18 @@
         <v>13</v>
       </c>
       <c r="O26" s="7" t="s">
-        <v>580</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>18</v>
@@ -9082,16 +9229,16 @@
         <v>13</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="M27" s="9" t="s">
         <v>12</v>
@@ -9100,18 +9247,18 @@
         <v>13</v>
       </c>
       <c r="O27" s="9" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="60" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>12</v>
@@ -9120,16 +9267,16 @@
         <v>13</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="J28" s="7" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>590</v>
+        <v>514</v>
       </c>
       <c r="L28" s="7" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="M28" s="7" t="s">
         <v>18</v>
@@ -9138,18 +9285,18 @@
         <v>27</v>
       </c>
       <c r="O28" s="7" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="75" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>18</v>
@@ -9158,16 +9305,16 @@
         <v>13</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="K29" s="17" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="M29" s="9" t="s">
         <v>18</v>
@@ -9176,18 +9323,18 @@
         <v>13</v>
       </c>
       <c r="O29" s="9" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="26.4" x14ac:dyDescent="0.25">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="45" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>18</v>
@@ -9196,18 +9343,18 @@
         <v>13</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="39.6" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D31" s="9" t="s">
         <v>12</v>
@@ -9216,26 +9363,28 @@
         <v>13</v>
       </c>
       <c r="F31" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="J31" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="22"/>
-      <c r="N31" s="22"/>
-      <c r="O31" s="22"/>
-    </row>
-    <row r="32" spans="1:15" ht="52.8" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="J31" s="9"/>
+      <c r="K31" s="17" t="s">
+        <v>593</v>
+      </c>
+      <c r="L31" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="M31" s="9"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="9"/>
+    </row>
+    <row r="32" spans="1:18" ht="75" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>18</v>
@@ -9244,18 +9393,28 @@
         <v>13</v>
       </c>
       <c r="F32" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="J32" s="9"/>
+      <c r="K32" s="17" t="s">
+        <v>594</v>
+      </c>
+      <c r="L32" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="M32" s="9"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="9"/>
+    </row>
+    <row r="33" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D33" s="9" t="s">
         <v>18</v>
@@ -9264,18 +9423,28 @@
         <v>13</v>
       </c>
       <c r="F33" s="9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="J33" s="9"/>
+      <c r="K33" s="17" t="s">
+        <v>595</v>
+      </c>
+      <c r="L33" s="9" t="s">
+        <v>599</v>
+      </c>
+      <c r="M33" s="9"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="9"/>
+    </row>
+    <row r="34" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C34" s="7" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>12</v>
@@ -9284,18 +9453,28 @@
         <v>13</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="J34" s="9"/>
+      <c r="K34" s="17" t="s">
+        <v>596</v>
+      </c>
+      <c r="L34" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="M34" s="9"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="9"/>
+    </row>
+    <row r="35" spans="1:15" ht="90" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D35" s="9" t="s">
         <v>18</v>
@@ -9304,18 +9483,28 @@
         <v>13</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="J35" s="9"/>
+      <c r="K35" s="17" t="s">
+        <v>601</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="M35" s="9"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="9"/>
+    </row>
+    <row r="36" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C36" s="7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>18</v>
@@ -9324,18 +9513,28 @@
         <v>13</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="J36" s="9"/>
+      <c r="K36" s="17" t="s">
+        <v>603</v>
+      </c>
+      <c r="L36" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="M36" s="9"/>
+      <c r="N36" s="10"/>
+      <c r="O36" s="9"/>
+    </row>
+    <row r="37" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D37" s="9" t="s">
         <v>12</v>
@@ -9344,18 +9543,28 @@
         <v>13</v>
       </c>
       <c r="F37" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="J37" s="9"/>
+      <c r="K37" s="17" t="s">
+        <v>604</v>
+      </c>
+      <c r="L37" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="M37" s="9"/>
+      <c r="N37" s="10"/>
+      <c r="O37" s="9"/>
+    </row>
+    <row r="38" spans="1:15" ht="90" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D38" s="7" t="s">
         <v>18</v>
@@ -9364,18 +9573,18 @@
         <v>13</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D39" s="9" t="s">
         <v>18</v>
@@ -9384,18 +9593,26 @@
         <v>13</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="J39" s="28" t="s">
+        <v>590</v>
+      </c>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+    </row>
+    <row r="40" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C40" s="7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D40" s="7" t="s">
         <v>12</v>
@@ -9404,18 +9621,18 @@
         <v>13</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="75" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D41" s="9" t="s">
         <v>18</v>
@@ -9424,18 +9641,26 @@
         <v>13</v>
       </c>
       <c r="F41" s="12" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="J41" s="29" t="s">
+        <v>592</v>
+      </c>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+    </row>
+    <row r="42" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B42" s="19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>18</v>
@@ -9444,18 +9669,18 @@
         <v>13</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>12</v>
@@ -9464,18 +9689,18 @@
         <v>13</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" ht="75" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D44" s="7" t="s">
         <v>18</v>
@@ -9484,18 +9709,18 @@
         <v>13</v>
       </c>
       <c r="F44" s="11" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B45" s="17" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D45" s="9" t="s">
         <v>18</v>
@@ -9504,18 +9729,18 @@
         <v>13</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>12</v>
@@ -9524,18 +9749,18 @@
         <v>13</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D47" s="9" t="s">
         <v>18</v>
@@ -9544,18 +9769,18 @@
         <v>13</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="60" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D48" s="7" t="s">
         <v>12</v>
@@ -9564,18 +9789,18 @@
         <v>13</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D49" s="9" t="s">
         <v>18</v>
@@ -9584,18 +9809,18 @@
         <v>13</v>
       </c>
       <c r="F49" s="9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D50" s="7" t="s">
         <v>12</v>
@@ -9604,18 +9829,18 @@
         <v>13</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>18</v>
@@ -9624,18 +9849,18 @@
         <v>13</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>12</v>
@@ -9644,18 +9869,18 @@
         <v>13</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B53" s="17" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C53" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D53" s="9" t="s">
         <v>18</v>
@@ -9664,18 +9889,18 @@
         <v>13</v>
       </c>
       <c r="F53" s="9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D54" s="7" t="s">
         <v>12</v>
@@ -9684,18 +9909,18 @@
         <v>13</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D55" s="9" t="s">
         <v>18</v>
@@ -9704,18 +9929,18 @@
         <v>13</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="C56" s="13" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>12</v>
@@ -9724,18 +9949,18 @@
         <v>13</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C57" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>18</v>
@@ -9744,18 +9969,18 @@
         <v>13</v>
       </c>
       <c r="F57" s="9" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D58" s="7" t="s">
         <v>12</v>
@@ -9764,18 +9989,18 @@
         <v>13</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B59" s="17" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C59" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>18</v>
@@ -9784,18 +10009,18 @@
         <v>13</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>12</v>
@@ -9804,18 +10029,18 @@
         <v>13</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C61" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D61" s="9" t="s">
         <v>18</v>
@@ -9824,18 +10049,18 @@
         <v>13</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C62" s="7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>12</v>
@@ -9844,18 +10069,18 @@
         <v>13</v>
       </c>
       <c r="F62" s="11" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C63" s="9" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D63" s="9" t="s">
         <v>12</v>
@@ -9864,18 +10089,18 @@
         <v>13</v>
       </c>
       <c r="F63" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>12</v>
@@ -9884,18 +10109,18 @@
         <v>13</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C65" s="9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D65" s="9" t="s">
         <v>12</v>
@@ -9904,18 +10129,18 @@
         <v>13</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B66" s="17" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D66" s="7" t="s">
         <v>12</v>
@@ -9924,18 +10149,18 @@
         <v>13</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="105" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B67" s="17" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="D67" s="9" t="s">
         <v>18</v>
@@ -9944,18 +10169,18 @@
         <v>13</v>
       </c>
       <c r="F67" s="12" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B68" s="17" t="s">
-        <v>253</v>
-      </c>
-      <c r="C68" s="7" t="s">
         <v>254</v>
+      </c>
+      <c r="C68" s="21" t="s">
+        <v>255</v>
       </c>
       <c r="D68" s="7" t="s">
         <v>18</v>
@@ -9964,18 +10189,18 @@
         <v>13</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B69" s="17" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C69" s="12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D69" s="9" t="s">
         <v>18</v>
@@ -9984,18 +10209,18 @@
         <v>13</v>
       </c>
       <c r="F69" s="12" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D70" s="7" t="s">
         <v>12</v>
@@ -10004,18 +10229,18 @@
         <v>13</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="105.6" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="120" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>18</v>
@@ -10024,18 +10249,18 @@
         <v>13</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C72" s="7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D72" s="7" t="s">
         <v>12</v>
@@ -10044,18 +10269,18 @@
         <v>13</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B73" s="17" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D73" s="9" t="s">
         <v>18</v>
@@ -10064,18 +10289,18 @@
         <v>13</v>
       </c>
       <c r="F73" s="12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A74" s="7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="B74" s="17" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D74" s="7" t="s">
         <v>18</v>
@@ -10084,18 +10309,18 @@
         <v>13</v>
       </c>
       <c r="F74" s="11" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="B75" s="17" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C75" s="12" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>18</v>
@@ -10104,18 +10329,18 @@
         <v>13</v>
       </c>
       <c r="F75" s="12" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A76" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="D76" s="7" t="s">
         <v>18</v>
@@ -10124,18 +10349,18 @@
         <v>13</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C77" s="12" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D77" s="9" t="s">
         <v>18</v>
@@ -10144,18 +10369,18 @@
         <v>13</v>
       </c>
       <c r="F77" s="12" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A78" s="7" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B78" s="17" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="D78" s="7" t="s">
         <v>18</v>
@@ -10164,18 +10389,18 @@
         <v>13</v>
       </c>
       <c r="F78" s="11" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A79" s="9" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B79" s="17" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>18</v>
@@ -10184,18 +10409,18 @@
         <v>13</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A80" s="7" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="D80" s="7" t="s">
         <v>18</v>
@@ -10204,18 +10429,18 @@
         <v>13</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="92.4" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="120" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B81" s="17" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>18</v>
@@ -10224,18 +10449,18 @@
         <v>13</v>
       </c>
       <c r="F81" s="12" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A82" s="7" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B82" s="17" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C82" s="7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D82" s="7" t="s">
         <v>18</v>
@@ -10244,18 +10469,18 @@
         <v>13</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C83" s="9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>12</v>
@@ -10264,18 +10489,18 @@
         <v>13</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A84" s="7" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B84" s="17" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C84" s="7" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D84" s="7" t="s">
         <v>18</v>
@@ -10284,18 +10509,18 @@
         <v>13</v>
       </c>
       <c r="F84" s="7" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A85" s="5" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>12</v>
@@ -10304,18 +10529,18 @@
         <v>13</v>
       </c>
       <c r="F85" s="16" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B86" s="17" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C86" s="7" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D86" s="7" t="s">
         <v>18</v>
@@ -10324,18 +10549,18 @@
         <v>13</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A87" s="9" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C87" s="12" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D87" s="9" t="s">
         <v>18</v>
@@ -10344,18 +10569,18 @@
         <v>13</v>
       </c>
       <c r="F87" s="9" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B88" s="7" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C88" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D88" s="7" t="s">
         <v>12</v>
@@ -10364,18 +10589,18 @@
         <v>13</v>
       </c>
       <c r="F88" s="7" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="B89" s="17" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C89" s="12" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D89" s="9" t="s">
         <v>18</v>
@@ -10384,18 +10609,18 @@
         <v>13</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C90" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D90" s="7" t="s">
         <v>12</v>
@@ -10404,18 +10629,18 @@
         <v>13</v>
       </c>
       <c r="F90" s="7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A91" s="9" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B91" s="17" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C91" s="12" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D91" s="9" t="s">
         <v>18</v>
@@ -10424,18 +10649,18 @@
         <v>13</v>
       </c>
       <c r="F91" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C92" s="7" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D92" s="7" t="s">
         <v>12</v>
@@ -10444,18 +10669,18 @@
         <v>13</v>
       </c>
       <c r="F92" s="7" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="90" x14ac:dyDescent="0.2">
       <c r="A93" s="9" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B93" s="17" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C93" s="12" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="D93" s="9" t="s">
         <v>18</v>
@@ -10464,18 +10689,18 @@
         <v>13</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="D94" s="7" t="s">
         <v>18</v>
@@ -10484,18 +10709,18 @@
         <v>13</v>
       </c>
       <c r="F94" s="7" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C95" s="9" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D95" s="9" t="s">
         <v>12</v>
@@ -10504,18 +10729,18 @@
         <v>13</v>
       </c>
       <c r="F95" s="9" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B96" s="17" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D96" s="7" t="s">
         <v>18</v>
@@ -10524,18 +10749,18 @@
         <v>13</v>
       </c>
       <c r="F96" s="7" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A97" s="9" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C97" s="9" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D97" s="9" t="s">
         <v>12</v>
@@ -10544,18 +10769,18 @@
         <v>13</v>
       </c>
       <c r="F97" s="9" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A98" s="7" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B98" s="17" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C98" s="11" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D98" s="7" t="s">
         <v>18</v>
@@ -10564,18 +10789,18 @@
         <v>13</v>
       </c>
       <c r="F98" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A99" s="5" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>12</v>
@@ -10584,18 +10809,18 @@
         <v>13</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A100" s="7" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B100" s="17" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C100" s="20" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D100" s="7" t="s">
         <v>18</v>
@@ -10604,18 +10829,18 @@
         <v>13</v>
       </c>
       <c r="F100" s="7" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="52.8" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="75" x14ac:dyDescent="0.2">
       <c r="A101" s="9" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B101" s="9" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C101" s="9" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>12</v>
@@ -10624,18 +10849,18 @@
         <v>13</v>
       </c>
       <c r="F101" s="9" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B102" s="17" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D102" s="7" t="s">
         <v>18</v>
@@ -10644,18 +10869,18 @@
         <v>13</v>
       </c>
       <c r="F102" s="7" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>12</v>
@@ -10664,18 +10889,18 @@
         <v>13</v>
       </c>
       <c r="F103" s="9" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="79.2" x14ac:dyDescent="0.25">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="105" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B104" s="17" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D104" s="7" t="s">
         <v>18</v>
@@ -10684,18 +10909,18 @@
         <v>13</v>
       </c>
       <c r="F104" s="7" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="105" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D105" s="9" t="s">
         <v>12</v>
@@ -10704,18 +10929,18 @@
         <v>13</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B106" s="17" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C106" s="7" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="D106" s="7" t="s">
         <v>18</v>
@@ -10724,18 +10949,18 @@
         <v>13</v>
       </c>
       <c r="F106" s="7" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B107" s="17" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="D107" s="9" t="s">
         <v>18</v>
@@ -10744,18 +10969,18 @@
         <v>13</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="7" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B108" s="17" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="C108" s="7" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="D108" s="7" t="s">
         <v>18</v>
@@ -10764,18 +10989,18 @@
         <v>13</v>
       </c>
       <c r="F108" s="7" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="9" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B109" s="17" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C109" s="7" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="D109" s="9" t="s">
         <v>18</v>
@@ -10784,18 +11009,18 @@
         <v>13</v>
       </c>
       <c r="F109" s="9" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C110" s="7" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>12</v>
@@ -10804,18 +11029,18 @@
         <v>13</v>
       </c>
       <c r="F110" s="7" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A111" s="9" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="D111" s="9" t="s">
         <v>12</v>
@@ -10824,18 +11049,18 @@
         <v>13</v>
       </c>
       <c r="F111" s="9" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A112" s="7" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="D112" s="7" t="s">
         <v>12</v>
@@ -10844,18 +11069,18 @@
         <v>13</v>
       </c>
       <c r="F112" s="7" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A113" s="9" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="D113" s="9" t="s">
         <v>12</v>
@@ -10864,18 +11089,18 @@
         <v>13</v>
       </c>
       <c r="F113" s="9" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A114" s="7" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C114" s="7" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="D114" s="7" t="s">
         <v>12</v>
@@ -10884,18 +11109,18 @@
         <v>13</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A115" s="9" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>12</v>
@@ -10904,18 +11129,18 @@
         <v>13</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A116" s="13" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C116" s="13" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="D116" s="13" t="s">
         <v>12</v>
@@ -10924,18 +11149,18 @@
         <v>13</v>
       </c>
       <c r="F116" s="13" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A117" s="9" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D117" s="9" t="s">
         <v>12</v>
@@ -10944,18 +11169,18 @@
         <v>13</v>
       </c>
       <c r="F117" s="9" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A118" s="7" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B118" s="7" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C118" s="7" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="D118" s="7" t="s">
         <v>12</v>
@@ -10964,18 +11189,18 @@
         <v>13</v>
       </c>
       <c r="F118" s="7" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A119" s="9" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>18</v>
@@ -10984,18 +11209,18 @@
         <v>13</v>
       </c>
       <c r="F119" s="9" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A120" s="7" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="B120" s="7" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C120" s="7" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D120" s="7" t="s">
         <v>18</v>
@@ -11004,18 +11229,18 @@
         <v>13</v>
       </c>
       <c r="F120" s="7" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A121" s="9" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>18</v>
@@ -11024,18 +11249,18 @@
         <v>13</v>
       </c>
       <c r="F121" s="9" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A122" s="7" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C122" s="7" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D122" s="7" t="s">
         <v>18</v>
@@ -11044,18 +11269,18 @@
         <v>13</v>
       </c>
       <c r="F122" s="7" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A123" s="9" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C123" s="9" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="D123" s="9" t="s">
         <v>18</v>
@@ -11064,18 +11289,18 @@
         <v>13</v>
       </c>
       <c r="F123" s="9" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A124" s="7" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B124" s="7" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C124" s="7" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="D124" s="7" t="s">
         <v>18</v>
@@ -11084,18 +11309,18 @@
         <v>13</v>
       </c>
       <c r="F124" s="7" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A125" s="9" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="D125" s="9" t="s">
         <v>18</v>
@@ -11104,18 +11329,18 @@
         <v>13</v>
       </c>
       <c r="F125" s="9" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A126" s="7" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B126" s="7" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C126" s="7" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D126" s="7" t="s">
         <v>18</v>
@@ -11124,18 +11349,18 @@
         <v>13</v>
       </c>
       <c r="F126" s="7" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A127" s="9" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>12</v>
@@ -11144,18 +11369,18 @@
         <v>13</v>
       </c>
       <c r="F127" s="9" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A128" s="7" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B128" s="7" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C128" s="7" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D128" s="7" t="s">
         <v>12</v>
@@ -11164,18 +11389,18 @@
         <v>13</v>
       </c>
       <c r="F128" s="7" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A129" s="9" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C129" s="9" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="D129" s="9" t="s">
         <v>12</v>
@@ -11184,18 +11409,18 @@
         <v>13</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A130" s="7" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B130" s="7" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C130" s="7" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D130" s="7" t="s">
         <v>12</v>
@@ -11204,18 +11429,18 @@
         <v>13</v>
       </c>
       <c r="F130" s="7" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A131" s="9" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="D131" s="9" t="s">
         <v>12</v>
@@ -11224,18 +11449,18 @@
         <v>13</v>
       </c>
       <c r="F131" s="9" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A132" s="7" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B132" s="7" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D132" s="7" t="s">
         <v>12</v>
@@ -11244,18 +11469,18 @@
         <v>13</v>
       </c>
       <c r="F132" s="7" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A133" s="9" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D133" s="9" t="s">
         <v>12</v>
@@ -11264,18 +11489,18 @@
         <v>13</v>
       </c>
       <c r="F133" s="9" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A134" s="7" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B134" s="7" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="D134" s="7" t="s">
         <v>12</v>
@@ -11284,18 +11509,18 @@
         <v>13</v>
       </c>
       <c r="F134" s="7" t="s">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.2">
       <c r="A135" s="9" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="D135" s="9" t="s">
         <v>12</v>
@@ -11304,18 +11529,18 @@
         <v>13</v>
       </c>
       <c r="F135" s="9" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A136" s="7" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B136" s="7" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D136" s="7" t="s">
         <v>12</v>
@@ -11324,18 +11549,18 @@
         <v>13</v>
       </c>
       <c r="F136" s="7" t="s">
-        <v>501</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A137" s="5" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B137" s="5" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C137" s="5" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="D137" s="5" t="s">
         <v>12</v>
@@ -11344,18 +11569,18 @@
         <v>13</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>504</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A138" s="7" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="B138" s="7" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="D138" s="7" t="s">
         <v>12</v>
@@ -11364,18 +11589,18 @@
         <v>13</v>
       </c>
       <c r="F138" s="7" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A139" s="9" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B139" s="17" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C139" s="9" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="D139" s="9" t="s">
         <v>12</v>
@@ -11384,18 +11609,18 @@
         <v>13</v>
       </c>
       <c r="F139" s="9" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A140" s="7" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B140" s="17" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="D140" s="7" t="s">
         <v>18</v>
@@ -11404,18 +11629,18 @@
         <v>27</v>
       </c>
       <c r="F140" s="7" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A141" s="9" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B141" s="17" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="D141" s="9" t="s">
         <v>18</v>
@@ -11424,37 +11649,41 @@
         <v>13</v>
       </c>
       <c r="F141" s="9" t="s">
-        <v>517</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A143" s="22" t="s">
-        <v>585</v>
-      </c>
-      <c r="B143" s="22"/>
-      <c r="C143" s="22"/>
-      <c r="D143" s="22"/>
-      <c r="E143" s="22"/>
-      <c r="F143" s="22"/>
-    </row>
-    <row r="145" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="A145" s="23" t="s">
-        <v>586</v>
-      </c>
-      <c r="B145" s="23"/>
-      <c r="C145" s="23"/>
-      <c r="D145" s="23"/>
-      <c r="E145" s="23"/>
-      <c r="F145" s="23"/>
+        <v>518</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A143" s="28" t="s">
+        <v>590</v>
+      </c>
+      <c r="B143" s="28"/>
+      <c r="C143" s="28"/>
+      <c r="D143" s="28"/>
+      <c r="E143" s="28"/>
+      <c r="F143" s="28"/>
+    </row>
+    <row r="145" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A145" s="30" t="s">
+        <v>591</v>
+      </c>
+      <c r="B145" s="30"/>
+      <c r="C145" s="30"/>
+      <c r="D145" s="30"/>
+      <c r="E145" s="30"/>
+      <c r="F145" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="J31:O31"/>
+  <mergeCells count="13">
+    <mergeCell ref="J39:O39"/>
     <mergeCell ref="A143:F143"/>
     <mergeCell ref="A145:F145"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:G3"/>
+    <mergeCell ref="J41:O41"/>
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="AA5:AB5"/>
     <mergeCell ref="J1:P1"/>
     <mergeCell ref="J2:O2"/>
     <mergeCell ref="J3:P3"/>

</xml_diff>

<commit_message>
actualizar carpeta de documentos
</commit_message>
<xml_diff>
--- a/document/Etiquetas.xlsx
+++ b/document/Etiquetas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\Dropbox\Facultad\UBA\Tercer trimestre\Machine Learning\ML_PS2_Falcone_Morales_Riverti\document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0E7CA2-B625-467B-84CA-17754D598315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40AE4924-EDD6-4A54-B645-75516513ABC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7504,8 +7504,11 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -7513,14 +7516,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8233,8 +8233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8256,62 +8256,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="J1" s="26" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="J1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="J2" s="27" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="J2" s="28" t="s">
         <v>519</v>
       </c>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
     </row>
     <row r="3" spans="1:28" ht="18" x14ac:dyDescent="0.2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="J3" s="26" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="J3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
-      <c r="N3" s="26"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
     </row>
     <row r="4" spans="1:28" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -8388,14 +8388,14 @@
       <c r="O5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="AA5" s="25"/>
-      <c r="AB5" s="25"/>
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="W5" s="30"/>
+      <c r="X5" s="30"/>
+      <c r="Y5" s="30"/>
+      <c r="AA5" s="30"/>
+      <c r="AB5" s="30"/>
     </row>
     <row r="6" spans="1:28" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
@@ -8547,7 +8547,7 @@
       <c r="K9" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="L9" s="9" t="s">
+      <c r="L9" s="21" t="s">
         <v>30</v>
       </c>
       <c r="M9" s="9" t="s">
@@ -9369,7 +9369,7 @@
       <c r="K31" s="17" t="s">
         <v>593</v>
       </c>
-      <c r="L31" s="9" t="s">
+      <c r="L31" s="21" t="s">
         <v>597</v>
       </c>
       <c r="M31" s="9"/>
@@ -9399,7 +9399,7 @@
       <c r="K32" s="17" t="s">
         <v>594</v>
       </c>
-      <c r="L32" s="9" t="s">
+      <c r="L32" s="21" t="s">
         <v>598</v>
       </c>
       <c r="M32" s="9"/>
@@ -9429,7 +9429,7 @@
       <c r="K33" s="17" t="s">
         <v>595</v>
       </c>
-      <c r="L33" s="9" t="s">
+      <c r="L33" s="21" t="s">
         <v>599</v>
       </c>
       <c r="M33" s="9"/>
@@ -9459,7 +9459,7 @@
       <c r="K34" s="17" t="s">
         <v>596</v>
       </c>
-      <c r="L34" s="9" t="s">
+      <c r="L34" s="21" t="s">
         <v>600</v>
       </c>
       <c r="M34" s="9"/>
@@ -9489,7 +9489,7 @@
       <c r="K35" s="17" t="s">
         <v>601</v>
       </c>
-      <c r="L35" s="9" t="s">
+      <c r="L35" s="21" t="s">
         <v>602</v>
       </c>
       <c r="M35" s="9"/>
@@ -9519,7 +9519,7 @@
       <c r="K36" s="17" t="s">
         <v>603</v>
       </c>
-      <c r="L36" s="9" t="s">
+      <c r="L36" s="21" t="s">
         <v>606</v>
       </c>
       <c r="M36" s="9"/>
@@ -9549,7 +9549,7 @@
       <c r="K37" s="17" t="s">
         <v>604</v>
       </c>
-      <c r="L37" s="9" t="s">
+      <c r="L37" s="21" t="s">
         <v>605</v>
       </c>
       <c r="M37" s="9"/>
@@ -9595,14 +9595,14 @@
       <c r="F39" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="J39" s="28" t="s">
+      <c r="J39" s="25" t="s">
         <v>590</v>
       </c>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="28"/>
-      <c r="O39" s="28"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
     </row>
     <row r="40" spans="1:15" ht="45" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
@@ -11653,27 +11653,33 @@
       </c>
     </row>
     <row r="143" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A143" s="28" t="s">
+      <c r="A143" s="25" t="s">
         <v>590</v>
       </c>
-      <c r="B143" s="28"/>
-      <c r="C143" s="28"/>
-      <c r="D143" s="28"/>
-      <c r="E143" s="28"/>
-      <c r="F143" s="28"/>
+      <c r="B143" s="25"/>
+      <c r="C143" s="25"/>
+      <c r="D143" s="25"/>
+      <c r="E143" s="25"/>
+      <c r="F143" s="25"/>
     </row>
     <row r="145" spans="1:6" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A145" s="30" t="s">
+      <c r="A145" s="26" t="s">
         <v>591</v>
       </c>
-      <c r="B145" s="30"/>
-      <c r="C145" s="30"/>
-      <c r="D145" s="30"/>
-      <c r="E145" s="30"/>
-      <c r="F145" s="30"/>
+      <c r="B145" s="26"/>
+      <c r="C145" s="26"/>
+      <c r="D145" s="26"/>
+      <c r="E145" s="26"/>
+      <c r="F145" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="S5:U5"/>
+    <mergeCell ref="W5:Y5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="J1:P1"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="J3:P3"/>
     <mergeCell ref="J39:O39"/>
     <mergeCell ref="A143:F143"/>
     <mergeCell ref="A145:F145"/>
@@ -11681,12 +11687,6 @@
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="J41:O41"/>
-    <mergeCell ref="S5:U5"/>
-    <mergeCell ref="W5:Y5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="J1:P1"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="J3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>